<commit_message>
Atualização do Boletim de Acompanhamento de Abril/2016, Relatório Mensal de Pagamentos referentes ao mês Maio/2016 e as atas de reuniões do comitê.
</commit_message>
<xml_diff>
--- a/00_GESTAO_GERAL/04_RELATORIO/Relatóro Mensal de Ordens de Serviços - 201605.xlsx
+++ b/00_GESTAO_GERAL/04_RELATORIO/Relatóro Mensal de Ordens de Serviços - 201605.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="142">
   <si>
     <t>Número OS</t>
   </si>
@@ -478,9 +478,6 @@
   </si>
   <si>
     <t>Produto Arrecadação - Subproduto Parametrização da Arrecadação Versão (1.0)</t>
-  </si>
-  <si>
-    <t>xxxx</t>
   </si>
   <si>
     <t>Produto Serviços Transversais - Subproduto Gestão de Segurança Básico Versão (1.0)</t>
@@ -1679,7 +1676,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD15"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,8 +1812,8 @@
       <c r="V2" s="21"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="s">
-        <v>140</v>
+      <c r="A3" s="21">
+        <v>4757</v>
       </c>
       <c r="B3" t="s">
         <v>74</v>
@@ -1828,12 +1825,14 @@
         <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F3" s="52">
         <v>42486</v>
       </c>
-      <c r="G3" s="52"/>
+      <c r="G3" s="52">
+        <v>42493</v>
+      </c>
       <c r="H3" s="52"/>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
@@ -1901,10 +1900,12 @@
       <c r="A1" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="64"/>
+      <c r="B1" s="64">
+        <v>42495</v>
+      </c>
       <c r="D1" s="62"/>
       <c r="E1" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F1" s="62"/>
       <c r="G1" s="62"/>
@@ -2448,9 +2449,9 @@
       <c r="P9" s="37"/>
     </row>
     <row r="10" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="54" t="str">
+      <c r="A10" s="54">
         <f>IF(ControleOSsMês!$G$1="Todas",IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($A$3)-1)/5)+1,1),""),IFERROR(VLOOKUP(INT((ROW()-ROW($A$3)-1)/5)+1,OSMês[],2,FALSE),""))</f>
-        <v>xxxx</v>
+        <v>4757</v>
       </c>
       <c r="B10" s="71" t="str">
         <f>IF(A10="","",VLOOKUP(A10,OSS[],MATCH("Situação da OS",OSS[#Headers],0),FALSE))</f>
@@ -2642,9 +2643,9 @@
         <v>84</v>
       </c>
       <c r="E12" s="37"/>
-      <c r="G12" s="20" t="str">
+      <c r="G12" s="20">
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Data de Inicio",OSS[#Headers],0),FALSE)))</f>
-        <v/>
+        <v>42493</v>
       </c>
       <c r="H12" s="20" t="str">
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("Entrega do Plano da OS",OSS[#Headers],0),FALSE)))</f>
@@ -2682,9 +2683,9 @@
         <f>IF(A10="","",IF(VLOOKUP(A10,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)="","",VLOOKUP(A10,OSS[],MATCH("PF Apurado",OSS[#Headers],0),FALSE)))</f>
         <v/>
       </c>
-      <c r="Q12" s="57" t="str">
-        <f>IF(F11="","",IF(G12="","",IF(L12="",IF(DataRef&lt;L11,L11,DataRef),L12)-L11))</f>
-        <v/>
+      <c r="Q12" s="57">
+        <f ca="1">IF(F11="","",IF(G12="","",IF(L12="",IF(DataRef&lt;L11,L11,DataRef),L12)-L11))</f>
+        <v>0</v>
       </c>
       <c r="R12" s="21" t="str">
         <f>IF(J12="","",AF11)</f>
@@ -2710,9 +2711,9 @@
         <f>IF(K12="","",AC12/IF($P12="",$P11,$P12))</f>
         <v/>
       </c>
-      <c r="X12" s="57" t="str">
-        <f ca="1">IF(F11="","",IF(G12="",IF(DataRef&lt;G11,"",DataRef-G11),G12-G11))</f>
-        <v/>
+      <c r="X12" s="57">
+        <f>IF(F11="","",IF(G12="",IF(DataRef&lt;G11,"",DataRef-G11),G12-G11))</f>
+        <v>0</v>
       </c>
       <c r="Y12" s="57" t="str">
         <f>IF(OR(R10="Hora Java",R10="Hora dotNet"),AG11,"")</f>
@@ -2774,7 +2775,7 @@
         <v/>
       </c>
       <c r="Q13" s="57" t="str">
-        <f>IF(Q12="","",IF(OR(Q11&gt;Q12,Z11&lt;Z12),"",ROUND(Q12*(IF($P12="",$P11,$P12)*SLA_ICA_EOS_Multa),2)))</f>
+        <f ca="1">IF(Q12="","",IF(OR(Q11&gt;Q12,Z11&lt;Z12),"",ROUND(Q12*(IF($P12="",$P11,$P12)*SLA_ICA_EOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="R13" s="57" t="str">
@@ -2802,7 +2803,7 @@
         <v/>
       </c>
       <c r="X13" s="57" t="str">
-        <f ca="1">IF(X12="","",IF(X11&gt;X12,"",ROUND(X12*(IF($P12="",$P11,$P12)*SLA_ICA_IOS_Multa),2)))</f>
+        <f>IF(X12="","",IF(X11&gt;X12,"",ROUND(X12*(IF($P12="",$P11,$P12)*SLA_ICA_IOS_Multa),2)))</f>
         <v/>
       </c>
       <c r="Y13" s="57" t="str">
@@ -14020,6 +14021,25 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B150:C150"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B135:C135"/>
+    <mergeCell ref="B140:C140"/>
+    <mergeCell ref="B145:C145"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B110:C110"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B5:C5"/>
@@ -14032,25 +14052,6 @@
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B150:C150"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B135:C135"/>
-    <mergeCell ref="B140:C140"/>
-    <mergeCell ref="B145:C145"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1">
@@ -14605,7 +14606,7 @@
       </c>
       <c r="H1" s="61" t="str">
         <f ca="1">YEAR(VALUE("01"&amp;"/"&amp;TEXT(MONTH(DataRef),"00")&amp;"/"&amp;YEAR(DataRef))-1)&amp;TEXT(MONTH(VALUE("01"&amp;"/"&amp;TEXT(MONTH(DataRef),"00")&amp;"/"&amp;YEAR(DataRef))-1),"00")</f>
-        <v>201603</v>
+        <v>201604</v>
       </c>
       <c r="I1" s="20"/>
       <c r="J1" t="s">
@@ -14613,21 +14614,21 @@
       </c>
       <c r="K1" s="20">
         <f ca="1">IF($L$1="",TODAY(),$L$1)</f>
-        <v>42486</v>
-      </c>
-      <c r="L1" s="52" t="str">
+        <v>42495</v>
+      </c>
+      <c r="L1" s="52">
         <f>IF(Mensal!B1="","",Mensal!B1)</f>
-        <v/>
+        <v>42495</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="21">
+      <c r="A2" s="21" t="str">
         <f t="shared" ref="A2:A15" ca="1" si="0">IF(E2=E1,"",E2)</f>
-        <v>1</v>
-      </c>
-      <c r="B2" s="21">
+        <v/>
+      </c>
+      <c r="B2" s="21" t="str">
         <f ca="1">IF(C2="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C2,""))</f>
-        <v>4721</v>
+        <v/>
       </c>
       <c r="C2" s="21">
         <f>IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($C$1)-1)/1)+1,1),"")</f>
@@ -14637,23 +14638,23 @@
         <f>IF(C2="","",VLOOKUP(C2,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>
         <v>42444</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="21" t="str">
         <f t="shared" ref="E2:E15" ca="1" si="1">IF(B2="",E1,IF(E1="",1,E1)+1)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="21" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="B3" s="21" t="str">
+      <c r="B3" s="21">
         <f ca="1">IF(C3="","",IF(YEAR(OSMês[[#This Row],[Data Situação]])&amp;TEXT(MONTH(OSMês[[#This Row],[Data Situação]]),"00")=$H$1,C3,""))</f>
-        <v/>
-      </c>
-      <c r="C3" s="21" t="str">
+        <v>4757</v>
+      </c>
+      <c r="C3" s="21">
         <f>IFERROR(INDEX(OSS[Número OS],INT((ROW()-ROW($C$1)-1)/1)+1,1),"")</f>
-        <v>xxxx</v>
+        <v>4757</v>
       </c>
       <c r="D3" s="52">
         <f>IF(C3="","",VLOOKUP(C3,OSS[],MATCH("Data Situação",OSS[#Headers],0),FALSE))</f>

</xml_diff>